<commit_message>
Data provider and listeners
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="DATA" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="29">
   <si>
     <t>testname</t>
   </si>
@@ -52,6 +52,57 @@
   </si>
   <si>
     <t>loginLogoutTest</t>
+  </si>
+  <si>
+    <t>testcasename</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>Niyaz</t>
+  </si>
+  <si>
+    <t>Subscribe</t>
+  </si>
+  <si>
+    <t>SeleniumAutomation</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>edge</t>
+  </si>
+  <si>
+    <t>To check whether Amazon website is working or not</t>
+  </si>
+  <si>
+    <t>menuItem</t>
+  </si>
+  <si>
+    <t>amazonHamburgerMenuTest</t>
+  </si>
+  <si>
+    <t>Power Banks</t>
   </si>
 </sst>
 </file>
@@ -384,15 +435,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -444,6 +495,23 @@
         <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -454,12 +522,183 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Driver code refactoring and docker compose file added
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -105,10 +105,10 @@
     <t>menuSubItem</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>YWRtaW4xMjM=</t>
+  </si>
+  <si>
+    <t>firefox</t>
   </si>
 </sst>
 </file>
@@ -531,7 +531,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -580,7 +580,7 @@
         <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
         <v>18</v>
@@ -603,7 +603,7 @@
         <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
@@ -626,7 +626,7 @@
         <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>21</v>
@@ -649,7 +649,7 @@
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>21</v>
@@ -672,7 +672,7 @@
         <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" t="s">
         <v>19</v>
@@ -732,10 +732,10 @@
         <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Page actions method added
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="30">
   <si>
     <t>testname</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>YWRtaW4xMjM=</t>
-  </si>
-  <si>
-    <t>firefox</t>
   </si>
   <si>
     <t>no</t>
@@ -531,7 +528,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -594,7 +591,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
         <v>22</v>
@@ -640,7 +637,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
         <v>23</v>
@@ -663,7 +660,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
@@ -712,7 +709,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>20</v>
@@ -732,10 +729,10 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
data provider utils updated
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="30">
   <si>
     <t>testname</t>
   </si>
@@ -441,7 +441,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -475,7 +475,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -492,7 +492,7 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>9</v>
@@ -525,10 +525,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -568,7 +568,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
         <v>22</v>
@@ -614,7 +614,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
         <v>23</v>
@@ -709,7 +709,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>20</v>
@@ -721,29 +721,6 @@
         <v>20</v>
       </c>
       <c r="G8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>